<commit_message>
adjusted files in BOM for voltage tolerance
</commit_message>
<xml_diff>
--- a/pcb/tritag/rev_c/tritag_bom.xlsx
+++ b/pcb/tritag/rev_c/tritag_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="273">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">SMD Capacitor</t>
   </si>
   <si>
-    <t xml:space="preserve">490-3083-1-ND</t>
+    <t xml:space="preserve">712-1266-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">1.2pF</t>
@@ -271,10 +271,10 @@
     <t xml:space="preserve">C69,C70</t>
   </si>
   <si>
-    <t xml:space="preserve">490-3896-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRM188R60J106ME47D </t>
+    <t xml:space="preserve">490-10474-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM188R61A106KE69D</t>
   </si>
   <si>
     <t xml:space="preserve">GREEN</t>
@@ -311,9 +311,6 @@
   </si>
   <si>
     <t xml:space="preserve">67-2125-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lumex Opto</t>
   </si>
   <si>
     <t xml:space="preserve">CON_MICRO_SDDM3AT-SF-PEJM5</t>
@@ -856,6 +853,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -877,6 +875,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -953,8 +952,8 @@
   </sheetPr>
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I56" activeCellId="0" sqref="I56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -963,11 +962,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.36"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="55.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="4.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.66"/>
@@ -1512,9 +1511,6 @@
       <c r="I21" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="J21" s="0" t="s">
-        <v>97</v>
-      </c>
       <c r="M21" s="0" t="s">
         <v>92</v>
       </c>
@@ -1524,22 +1520,22 @@
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="D22" s="0" t="s">
+      <c r="E22" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="F22" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="I22" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1547,25 +1543,25 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" s="0" t="s">
+      <c r="E23" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="F23" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="I23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="M23" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="M23" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,25 +1569,25 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>110</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>28</v>
       </c>
       <c r="E24" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="I24" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="M24" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="M24" s="0" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1599,25 +1595,25 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>28</v>
       </c>
       <c r="E25" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="I25" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="F25" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="I25" s="0" t="s">
+      <c r="M25" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="M25" s="0" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,25 +1621,25 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>120</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>81</v>
       </c>
       <c r="E26" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="I26" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="F26" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="I26" s="0" t="s">
+      <c r="M26" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="M26" s="0" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1654,22 +1650,22 @@
         <v>0</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="E27" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="F27" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="I27" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="M27" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="M27" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,22 +1676,22 @@
         <v>270</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>125</v>
-      </c>
       <c r="E28" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I28" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="F28" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I28" s="0" t="s">
+      <c r="M28" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="M28" s="0" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1706,19 +1702,19 @@
         <v>470</v>
       </c>
       <c r="C29" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>125</v>
-      </c>
       <c r="E29" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I29" s="0" t="s">
         <v>133</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1726,22 +1722,22 @@
         <v>4</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="E30" s="0" t="s">
+      <c r="F30" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I30" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1749,22 +1745,22 @@
         <v>1</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="E31" s="0" t="s">
+      <c r="F31" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I31" s="0" t="s">
         <v>139</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,22 +1768,22 @@
         <v>3</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="E32" s="0" t="s">
+      <c r="F32" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I32" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,22 +1791,22 @@
         <v>2</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="E33" s="0" t="s">
+      <c r="F33" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I33" s="0" t="s">
         <v>145</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I33" s="0" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,22 +1814,22 @@
         <v>1</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C34" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="E34" s="0" t="s">
+      <c r="F34" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I34" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1841,22 +1837,22 @@
         <v>3</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="E35" s="0" t="s">
+      <c r="F35" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I35" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1864,22 +1860,22 @@
         <v>1</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="E36" s="0" t="s">
+      <c r="F36" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I36" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1887,22 +1883,22 @@
         <v>1</v>
       </c>
       <c r="B37" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E37" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="C37" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="E37" s="0" t="s">
+      <c r="F37" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I37" s="0" t="s">
         <v>157</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,37 +1906,37 @@
         <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D38" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="C38" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="D38" s="0" t="s">
+      <c r="E38" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="F38" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="G38" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="G38" s="0" t="s">
+      <c r="H38" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="H38" s="0" t="s">
+      <c r="I38" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="I38" s="0" t="s">
+      <c r="J38" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="J38" s="0" t="s">
+      <c r="L38" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="L38" s="0" t="s">
-        <v>167</v>
-      </c>
       <c r="M38" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1948,34 +1944,34 @@
         <v>1</v>
       </c>
       <c r="B39" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D39" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="C39" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="D39" s="0" t="s">
+      <c r="E39" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="F39" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="F39" s="0" t="s">
+      <c r="G39" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="G39" s="0" t="s">
+      <c r="H39" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="H39" s="0" t="s">
+      <c r="I39" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="I39" s="0" t="s">
+      <c r="J39" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="J39" s="0" t="s">
+      <c r="M39" s="0" t="s">
         <v>175</v>
-      </c>
-      <c r="M39" s="0" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1983,31 +1979,31 @@
         <v>1</v>
       </c>
       <c r="B40" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D40" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="C40" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="D40" s="0" t="s">
+      <c r="E40" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="F40" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="F40" s="0" t="s">
+      <c r="I40" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="I40" s="0" t="s">
-        <v>181</v>
-      </c>
       <c r="M40" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O40" s="0" t="n">
         <v>1146033</v>
       </c>
       <c r="P40" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2015,31 +2011,31 @@
         <v>1</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="D41" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="C41" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="D41" s="0" t="s">
+      <c r="E41" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="F41" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="F41" s="0" t="s">
+      <c r="I41" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="I41" s="0" t="s">
+      <c r="J41" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="J41" s="0" t="s">
+      <c r="L41" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="L41" s="0" t="s">
+      <c r="M41" s="0" t="s">
         <v>189</v>
-      </c>
-      <c r="M41" s="0" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2047,34 +2043,34 @@
         <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="D42" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="C42" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="D42" s="0" t="s">
+      <c r="E42" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="F42" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="F42" s="0" t="s">
+      <c r="G42" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="G42" s="0" t="s">
+      <c r="H42" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="H42" s="0" t="s">
+      <c r="I42" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="I42" s="0" t="s">
+      <c r="J42" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="J42" s="0" t="s">
+      <c r="M42" s="0" t="s">
         <v>198</v>
-      </c>
-      <c r="M42" s="0" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2082,22 +2078,22 @@
         <v>1</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="D43" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="C43" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="D43" s="0" t="s">
+      <c r="E43" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="E43" s="0" t="s">
+      <c r="F43" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="F43" s="0" t="s">
+      <c r="I43" s="0" t="s">
         <v>203</v>
-      </c>
-      <c r="I43" s="0" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2105,37 +2101,37 @@
         <v>1</v>
       </c>
       <c r="B44" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="D44" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="C44" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="D44" s="0" t="s">
+      <c r="E44" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="F44" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="F44" s="0" t="s">
+      <c r="G44" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="G44" s="0" t="s">
+      <c r="H44" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="H44" s="0" t="s">
+      <c r="I44" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="I44" s="0" t="s">
+      <c r="J44" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="J44" s="0" t="s">
+      <c r="L44" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="L44" s="0" t="s">
+      <c r="M44" s="0" t="s">
         <v>213</v>
-      </c>
-      <c r="M44" s="0" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2143,28 +2139,28 @@
         <v>1</v>
       </c>
       <c r="B45" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="D45" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="C45" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="D45" s="0" t="s">
+      <c r="E45" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="F45" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="F45" s="0" t="s">
+      <c r="I45" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="I45" s="0" t="s">
+      <c r="J45" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="J45" s="0" t="s">
-        <v>220</v>
-      </c>
       <c r="M45" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2172,28 +2168,28 @@
         <v>1</v>
       </c>
       <c r="B46" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="D46" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="D46" s="0" t="s">
+      <c r="E46" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="F46" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="F46" s="0" t="s">
+      <c r="I46" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="I46" s="0" t="s">
+      <c r="J46" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="J46" s="0" t="s">
+      <c r="M46" s="0" t="s">
         <v>226</v>
-      </c>
-      <c r="M46" s="0" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2201,34 +2197,34 @@
         <v>1</v>
       </c>
       <c r="B47" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="D47" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="C47" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="D47" s="0" t="s">
+      <c r="E47" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="F47" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="F47" s="0" t="s">
+      <c r="G47" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="G47" s="0" t="s">
+      <c r="H47" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="H47" s="0" t="s">
+      <c r="I47" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="I47" s="0" t="s">
+      <c r="J47" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="J47" s="0" t="s">
+      <c r="M47" s="0" t="s">
         <v>235</v>
-      </c>
-      <c r="M47" s="0" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2236,37 +2232,37 @@
         <v>1</v>
       </c>
       <c r="B48" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="D48" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="C48" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="D48" s="0" t="s">
+      <c r="E48" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="E48" s="0" t="s">
+      <c r="F48" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="F48" s="0" t="s">
+      <c r="G48" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="G48" s="0" t="s">
+      <c r="H48" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="H48" s="0" t="s">
+      <c r="I48" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="I48" s="0" t="s">
+      <c r="J48" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="L48" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="J48" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="L48" s="0" t="s">
+      <c r="M48" s="0" t="s">
         <v>244</v>
-      </c>
-      <c r="M48" s="0" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2274,28 +2270,28 @@
         <v>1</v>
       </c>
       <c r="B49" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="C49" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="D49" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="E49" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="E49" s="0" t="s">
+      <c r="F49" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="F49" s="0" t="s">
+      <c r="I49" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="I49" s="0" t="s">
+      <c r="J49" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="J49" s="0" t="s">
+      <c r="M49" s="0" t="s">
         <v>252</v>
-      </c>
-      <c r="M49" s="0" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2303,31 +2299,31 @@
         <v>1</v>
       </c>
       <c r="B50" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="C50" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="D50" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="E50" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="E50" s="0" t="s">
+      <c r="F50" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="F50" s="0" t="s">
+      <c r="G50" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="G50" s="0" t="s">
+      <c r="H50" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="H50" s="0" t="s">
+      <c r="I50" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="I50" s="2" t="s">
+      <c r="J50" s="0" t="s">
         <v>260</v>
-      </c>
-      <c r="J50" s="0" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2335,28 +2331,28 @@
         <v>1</v>
       </c>
       <c r="B51" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="C51" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="D51" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="E51" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="F51" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="F51" s="0" t="s">
+      <c r="I51" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="I51" s="2" t="s">
+      <c r="J51" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="J51" s="0" t="s">
+      <c r="M51" s="0" t="s">
         <v>268</v>
-      </c>
-      <c r="M51" s="0" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2364,31 +2360,31 @@
         <v>1</v>
       </c>
       <c r="B52" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="E52" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="C52" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="E52" s="0" t="s">
+      <c r="F52" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="H52" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="F52" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="G52" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="H52" s="0" t="s">
+      <c r="I52" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="I52" s="0" t="s">
-        <v>273</v>
-      </c>
       <c r="J52" s="0" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>